<commit_message>
MIDI Learn specific CC
Also explored CC outputs on note change to confirm new note wait.  Removed as they stopped other notes triggering.
Occasionally a grace note or trill will be missed due to the wait.
</commit_message>
<xml_diff>
--- a/Sax_Fingering_details.xlsx
+++ b/Sax_Fingering_details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\Documents\GitHub\MIDI-Wind-Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D56A3E9-4982-4F98-8261-44209822D016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF89A73-932C-446F-B66A-EF2E7B01359E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{37DECD7E-2A26-408F-B389-C3EB14E31A56}"/>
+    <workbookView xWindow="29355" yWindow="240" windowWidth="26775" windowHeight="16260" activeTab="2" xr2:uid="{37DECD7E-2A26-408F-B389-C3EB14E31A56}"/>
   </bookViews>
   <sheets>
     <sheet name="Leonardo" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="88">
   <si>
     <t>C#</t>
   </si>
@@ -292,6 +292,15 @@
   </si>
   <si>
     <t>16va</t>
+  </si>
+  <si>
+    <t>Learn CC1</t>
+  </si>
+  <si>
+    <t>Learn CC2</t>
+  </si>
+  <si>
+    <t>MIDI</t>
   </si>
 </sst>
 </file>
@@ -1884,6 +1893,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1891,7 +1901,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2822,8 +2831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00263F9-C8C7-42DF-8462-CEECFF97E7F1}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5876,15 +5885,16 @@
   <dimension ref="A1:W59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M58" sqref="M58"/>
+      <selection pane="bottomRight" activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -7097,6 +7107,9 @@
       <c r="A42" s="5" t="s">
         <v>61</v>
       </c>
+      <c r="K42" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -7123,7 +7136,13 @@
       <c r="I43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="L43" t="s">
+      <c r="K43" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S43" t="s">
         <v>82</v>
       </c>
     </row>
@@ -7152,7 +7171,13 @@
       <c r="I44" s="3">
         <v>0</v>
       </c>
-      <c r="L44">
+      <c r="K44" s="3">
+        <v>0</v>
+      </c>
+      <c r="L44" s="3">
+        <v>0</v>
+      </c>
+      <c r="S44">
         <v>14</v>
       </c>
     </row>
@@ -7181,7 +7206,13 @@
       <c r="I45" s="3">
         <v>0</v>
       </c>
+      <c r="K45" s="3">
+        <v>1</v>
+      </c>
       <c r="L45" s="3">
+        <v>0</v>
+      </c>
+      <c r="S45" s="3">
         <v>12</v>
       </c>
     </row>
@@ -7208,7 +7239,13 @@
       <c r="I46" s="3">
         <v>0</v>
       </c>
-      <c r="L46" s="3">
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="S46" s="3">
         <v>11</v>
       </c>
     </row>
@@ -7237,7 +7274,13 @@
       <c r="I47" s="2">
         <v>0</v>
       </c>
+      <c r="K47" s="2">
+        <v>0</v>
+      </c>
       <c r="L47" s="2">
+        <v>0</v>
+      </c>
+      <c r="S47" s="2">
         <v>10</v>
       </c>
     </row>
@@ -7266,11 +7309,17 @@
       <c r="I48" s="3">
         <v>0</v>
       </c>
+      <c r="K48" s="3">
+        <v>0</v>
+      </c>
       <c r="L48" s="3">
+        <v>0</v>
+      </c>
+      <c r="S48" s="3">
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>71</v>
       </c>
@@ -7290,11 +7339,17 @@
       <c r="I49" s="3">
         <v>0</v>
       </c>
+      <c r="K49" s="3">
+        <v>0</v>
+      </c>
       <c r="L49" s="3">
+        <v>0</v>
+      </c>
+      <c r="S49" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>24</v>
       </c>
@@ -7319,11 +7374,17 @@
       <c r="I50" s="3">
         <v>0</v>
       </c>
+      <c r="K50" s="3">
+        <v>0</v>
+      </c>
       <c r="L50" s="3">
+        <v>0</v>
+      </c>
+      <c r="S50" s="3">
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>7</v>
       </c>
@@ -7348,11 +7409,17 @@
       <c r="I51" s="2">
         <v>0</v>
       </c>
-      <c r="L51" s="3">
+      <c r="K51" s="3">
+        <v>0</v>
+      </c>
+      <c r="L51" s="2">
+        <v>0</v>
+      </c>
+      <c r="S51" s="3">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
@@ -7377,11 +7444,17 @@
       <c r="I52" s="2">
         <v>0</v>
       </c>
-      <c r="L52" s="3">
+      <c r="K52" s="3">
+        <v>0</v>
+      </c>
+      <c r="L52" s="2">
+        <v>0</v>
+      </c>
+      <c r="S52" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
@@ -7406,11 +7479,17 @@
       <c r="I53" s="2">
         <v>0</v>
       </c>
-      <c r="L53" s="3">
+      <c r="K53" s="3">
+        <v>0</v>
+      </c>
+      <c r="L53" s="2">
+        <v>0</v>
+      </c>
+      <c r="S53" s="3">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>68</v>
       </c>
@@ -7435,12 +7514,18 @@
       <c r="I54" s="1">
         <v>1</v>
       </c>
-      <c r="L54" s="3">
+      <c r="K54" s="3">
+        <v>0</v>
+      </c>
+      <c r="L54" s="1">
+        <v>0</v>
+      </c>
+      <c r="M54" s="1"/>
+      <c r="S54" s="3">
         <v>20</v>
       </c>
-      <c r="M54" s="1"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>1</v>
       </c>
@@ -7462,11 +7547,17 @@
       <c r="I55" s="2">
         <v>0</v>
       </c>
-      <c r="L55" s="3">
+      <c r="K55" s="3">
+        <v>0</v>
+      </c>
+      <c r="L55" s="2">
+        <v>0</v>
+      </c>
+      <c r="S55" s="3">
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>76</v>
       </c>
@@ -7479,11 +7570,17 @@
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
-      <c r="L56" s="3">
+      <c r="K56" s="3">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="S56" s="3">
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>73</v>
       </c>
@@ -7493,11 +7590,17 @@
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
-      <c r="L57" s="3">
+      <c r="K57" s="3">
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="S57" s="3">
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>75</v>
       </c>
@@ -7507,11 +7610,17 @@
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
-      <c r="L58" s="3">
+      <c r="K58" s="3">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="S58" s="3">
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>81</v>
       </c>
@@ -7520,7 +7629,7 @@
         <v>4096</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" ref="C59:E59" si="4">C44*1+C45*2+C46*4+C47*8+C48*16+C49*32+C50*64+C51*128+C52*256+C53*512+C54*1024+C55*2048+C56*4096</f>
+        <f t="shared" ref="C59" si="4">C44*1+C45*2+C46*4+C47*8+C48*16+C49*32+C50*64+C51*128+C52*256+C53*512+C54*1024+C55*2048+C56*4096</f>
         <v>32</v>
       </c>
       <c r="D59" s="1">
@@ -7541,12 +7650,20 @@
         <v>2048</v>
       </c>
       <c r="I59" s="1">
-        <f t="shared" ref="I59" si="6">I44*1+I45*2+I46*4+I47*8+I48*16+I49*32+I50*64+I51*128+I52*256+I53*512+I54*1024+I55*2048+I56*4096</f>
+        <f t="shared" ref="I59:L59" si="6">I44*1+I45*2+I46*4+I47*8+I48*16+I49*32+I50*64+I51*128+I52*256+I53*512+I54*1024+I55*2048+I56*4096</f>
         <v>1024</v>
       </c>
+      <c r="K59" s="1">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="L59" s="1">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G28:J39 L28:S39 K29 K32 B28:C39 E28:E39">
+  <conditionalFormatting sqref="B28:C39 E28:E39 G28:J39 L28:S39 K29 K32">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -7562,7 +7679,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:O14 L45:L58">
+  <conditionalFormatting sqref="B3:O14 S45:S58">
     <cfRule type="cellIs" dxfId="3" priority="9" operator="lessThan">
       <formula>1</formula>
     </cfRule>
@@ -7570,7 +7687,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G44:I58">
+  <conditionalFormatting sqref="G44:I58 K47:K58 L47:L55 K44:L45">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>